<commit_message>
V1.0 (up & down buttons, segment store)
</commit_message>
<xml_diff>
--- a/e.g. file spier/SPIER_1_MAJOR_DAILY (2).xlsx
+++ b/e.g. file spier/SPIER_1_MAJOR_DAILY (2).xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7dc01f91e43520c4/Documenten/HMSM/Jaar 4/Intership/JUYO/.Converter/e.g. file spier/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_BB4E857E34DFFC8B1EF97A4630F5CD4C683E36D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7D4DF5-6C5E-4F0C-B9EF-49EF49DDDEA2}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView minimized="1" xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet0" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>DATE</t>
   </si>
@@ -69,16 +77,18 @@
   </si>
   <si>
     <t>HOUSE_USE_REV</t>
+  </si>
+  <si>
+    <t>JUYO Forecasting formatter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -90,7 +100,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -108,39 +118,348 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.98828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="22.9921875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="24.03515625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="26.046875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="27.08984375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="22.015625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="23.0546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="19.9375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="20.9765625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="21.7265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="22.76953125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="19.765625" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="20.8046875" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="15.83203125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="16.875" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="20.45703125" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="21.49609375" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="15.671875" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="16.7109375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -199,7 +518,12 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V1.1 (Fuzzy search added, started converting proce
</commit_message>
<xml_diff>
--- a/e.g. file spier/SPIER_1_MAJOR_DAILY (2).xlsx
+++ b/e.g. file spier/SPIER_1_MAJOR_DAILY (2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7dc01f91e43520c4/Documenten/HMSM/Jaar 4/Intership/JUYO/.Converter/e.g. file spier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_BB4E857E34DFFC8B1EF97A4630F5CD4C683E36D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7D4DF5-6C5E-4F0C-B9EF-49EF49DDDEA2}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_BB4E857E34DFFC8B1EF97A4630F5CD4C683E36D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AE2A29C-39F0-4FDA-B47E-B020D4E77C9B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="3630" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>DATE</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>HOUSE_USE_REV</t>
-  </si>
-  <si>
-    <t>JUYO Forecasting formatter</t>
   </si>
 </sst>
 </file>
@@ -132,6 +129,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,9 +433,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -518,11 +521,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V1.4 (General converter process done)
</commit_message>
<xml_diff>
--- a/e.g. file spier/SPIER_1_MAJOR_DAILY (2).xlsx
+++ b/e.g. file spier/SPIER_1_MAJOR_DAILY (2).xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7dc01f91e43520c4/Documenten/HMSM/Jaar 4/Intership/JUYO/.Converter/e.g. file spier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_BB4E857E34DFFC8B1EF97A4630F5CD4C683E36D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AE2A29C-39F0-4FDA-B47E-B020D4E77C9B}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_BB4E857E34DFFC8B1EF97A4630F5CD4C683E36D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABEC1308-4910-434D-AC52-FDA1A3FB73E9}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="3630" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2730" yWindow="2850" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -83,6 +96,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,15 +450,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
@@ -521,6 +538,282 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>